<commit_message>
Fix-banred-backsub, fix axiales, FIX EA, FINAL PROGRAM
</commit_message>
<xml_diff>
--- a/datos/3d/datos.xlsx
+++ b/datos/3d/datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\3d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12ED67B-5FED-4444-8468-F2D1ECD7F786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B34CB1-2CD3-4CFB-970A-070FEB8AC9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="11010" windowHeight="12885" firstSheet="1" activeTab="3" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>DIM</t>
   </si>
@@ -80,22 +80,13 @@
     <t>FZ [kN]</t>
   </si>
   <si>
-    <t>Nodo Restringido</t>
-  </si>
-  <si>
-    <t>Nodo Libre</t>
-  </si>
-  <si>
     <t>Agregar el valor de dimensión (1, 2 o 3)</t>
   </si>
   <si>
-    <t>E en GPA (kN/mm^2)</t>
-  </si>
-  <si>
-    <t>A en cm^2</t>
-  </si>
-  <si>
-    <t>AE en 10⁵N (100 kN).</t>
+    <t>Restringido</t>
+  </si>
+  <si>
+    <t>Libre</t>
   </si>
   <si>
     <t>A (cm^2)</t>
@@ -162,16 +153,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +506,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +523,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
@@ -537,7 +534,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
@@ -548,7 +545,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4">
@@ -559,7 +556,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5">
@@ -570,7 +567,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6">
@@ -581,7 +578,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7">
@@ -593,73 +590,45 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -673,15 +642,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -709,8 +678,21 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -738,8 +720,11 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -767,15 +752,8 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -803,15 +781,8 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -840,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -851,7 +822,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -862,7 +833,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -873,7 +844,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -884,7 +855,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -895,7 +866,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -906,7 +877,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -917,7 +888,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -930,8 +901,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -939,27 +910,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E1F06C-A87F-45D7-8D75-0575F1BF82DF}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -969,23 +938,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -993,38 +962,29 @@
         <v>8400</v>
       </c>
       <c r="C2" s="1">
-        <v>27.977499999999999</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>200</v>
+        <v>8400</v>
       </c>
       <c r="C3" s="1">
-        <v>27.977499999999999</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>300</v>
+        <v>8400</v>
       </c>
       <c r="C4" s="1">
-        <v>27.977499999999999</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>